<commit_message>
Added tech-folder JAP Submersive Fleet Corrected some commders id's Deleted GERMAN translation. Is gonna be a submod
</commit_message>
<xml_diff>
--- a/BICE modfile/Leader_ID.xlsx
+++ b/BICE modfile/Leader_ID.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GER" sheetId="1" r:id="rId1"/>
     <sheet name="ENG" sheetId="4" r:id="rId2"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId3"/>
+    <sheet name="USA" sheetId="5" r:id="rId3"/>
+    <sheet name="SOV" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="161">
   <si>
     <t>ID</t>
   </si>
@@ -439,12 +440,72 @@
   </si>
   <si>
     <t>Leese, Oliver</t>
+  </si>
+  <si>
+    <t>UNITED KINGDOM  400 - 599</t>
+  </si>
+  <si>
+    <t>Bradley, Omar</t>
+  </si>
+  <si>
+    <t>Eisenhower, Dwight D.</t>
+  </si>
+  <si>
+    <t>Patton, George S.</t>
+  </si>
+  <si>
+    <t>Keyes, Geoffrey</t>
+  </si>
+  <si>
+    <t>Truscott, Lucian</t>
+  </si>
+  <si>
+    <t>UNITED KINGDOM  600 - 799</t>
+  </si>
+  <si>
+    <t>Zhukov, Georgy</t>
+  </si>
+  <si>
+    <t>Rokossovsky, Konstantin</t>
+  </si>
+  <si>
+    <t>Vasilevsky, Aleksandr</t>
+  </si>
+  <si>
+    <t>Konev, Ivan</t>
+  </si>
+  <si>
+    <t>Timoshenko, Semyon</t>
+  </si>
+  <si>
+    <t>Voroshilov, Kliment</t>
+  </si>
+  <si>
+    <t>Tukhachevsky, Mikhail</t>
+  </si>
+  <si>
+    <t>Kasatonov, Vladimir</t>
+  </si>
+  <si>
+    <t>Golovko, Arseniy</t>
+  </si>
+  <si>
+    <t>Levchenko, Gordey</t>
+  </si>
+  <si>
+    <t>Gorshkov, Sergey</t>
+  </si>
+  <si>
+    <t>Shaposhnikov, Boris</t>
+  </si>
+  <si>
+    <t>Vlasov, Andrey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -510,6 +571,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -519,6 +583,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -567,7 +634,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,9 +667,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,6 +719,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -813,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
@@ -833,28 +934,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2253,7 +2354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -2273,17 +2374,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -3272,12 +3373,1956 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>400</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>401</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>402</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>403</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>404</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>405</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>406</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>407</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>408</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>409</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>410</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>411</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>412</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>413</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>414</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>415</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>416</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>417</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>418</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>419</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>420</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>421</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>422</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>423</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>424</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>425</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>426</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>427</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>428</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>429</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>430</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>431</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>432</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>433</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>434</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>435</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>436</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>437</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>438</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>439</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>440</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>441</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>442</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>443</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>444</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>445</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>446</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>447</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>448</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>449</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>450</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>451</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>452</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>453</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>454</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>455</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>456</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>457</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>458</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>459</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>460</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>461</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>462</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>463</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>464</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>465</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>466</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>467</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>468</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>469</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>470</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>471</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>472</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>473</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>474</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>475</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>476</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>477</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>478</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>479</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>480</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>481</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>482</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>483</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>484</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>485</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>486</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>487</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>488</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>489</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>490</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>491</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>492</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>493</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>494</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>495</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>496</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>497</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>498</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>499</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S107"/>
+  <sheetViews>
+    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>600</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>601</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>602</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>603</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>604</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>605</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>606</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>607</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>608</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>609</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>610</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>611</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>612</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>613</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>614</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>615</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>616</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>617</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>618</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>619</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>620</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>621</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>622</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>623</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>624</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>625</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>626</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>627</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>628</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>629</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>630</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>631</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>632</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>633</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>634</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>635</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>636</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>637</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>638</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>639</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>640</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>641</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>642</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>643</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>644</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>645</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>646</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>647</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>648</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>649</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>650</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>651</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>652</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>653</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>654</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>655</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>656</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>657</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>658</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>659</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>660</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>661</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>662</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>663</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>664</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>665</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>666</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>667</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>668</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>669</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>670</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>671</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>672</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>673</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>674</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>675</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>676</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>677</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>678</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>679</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>680</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>681</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>682</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>683</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>684</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>685</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>686</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>687</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>688</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>689</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>690</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>691</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>692</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>693</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>694</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>695</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>696</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>697</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>698</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>699</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New version 2.5.9 Enhanced line of the techtrees
</commit_message>
<xml_diff>
--- a/BICE modfile/Leader_ID.xlsx
+++ b/BICE modfile/Leader_ID.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="4440" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="GER" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="164">
   <si>
     <t>ID</t>
   </si>
@@ -500,6 +500,15 @@
   </si>
   <si>
     <t>Vlasov, Andrey</t>
+  </si>
+  <si>
+    <t>Bader, Paul</t>
+  </si>
+  <si>
+    <t>FM in 1941</t>
+  </si>
+  <si>
+    <t>FM in 1940</t>
   </si>
 </sst>
 </file>
@@ -594,7 +603,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -632,7 +641,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -738,7 +747,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -914,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1013,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="K4" s="2">
         <v>200</v>
@@ -1026,7 +1038,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="K5" s="2">
         <v>201</v>
@@ -1430,6 +1445,12 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K23" s="2">
         <v>219</v>
@@ -4333,7 +4354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ENG general skills done. WIP navyleaders ID. SOV start correcetd new ID's in countryfile and event.
</commit_message>
<xml_diff>
--- a/BICE modfile/Leader_ID.xlsx
+++ b/BICE modfile/Leader_ID.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="6540" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GER" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="USA" sheetId="5" r:id="rId3"/>
     <sheet name="SOV" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -376,9 +376,6 @@
     <t>Heer / Luftwaffe</t>
   </si>
   <si>
-    <t>UNITED KINGDOM  300 - 399</t>
-  </si>
-  <si>
     <t>Army / Airforce</t>
   </si>
   <si>
@@ -515,12 +512,15 @@
   </si>
   <si>
     <t>Resinged on 27 jan 1938</t>
+  </si>
+  <si>
+    <t>UNITED KINGDOM  300 - 700</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -591,7 +591,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -607,7 +607,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -649,7 +649,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -682,26 +682,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -734,23 +717,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -929,7 +895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -1022,7 +988,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K4" s="2">
         <v>200</v>
@@ -1047,7 +1013,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K5" s="2">
         <v>201</v>
@@ -1453,7 +1419,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>10</v>
@@ -1476,13 +1442,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K24" s="2">
         <v>220</v>
@@ -2390,8 +2356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2411,7 +2377,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2451,7 +2417,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2467,7 +2433,7 @@
         <v>300</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -2481,7 +2447,7 @@
         <v>301</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -2495,7 +2461,7 @@
         <v>302</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -2509,7 +2475,7 @@
         <v>303</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -2523,7 +2489,7 @@
         <v>304</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -2537,7 +2503,7 @@
         <v>305</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -2551,7 +2517,7 @@
         <v>306</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>10</v>
@@ -2565,7 +2531,7 @@
         <v>307</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -2579,7 +2545,7 @@
         <v>308</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
@@ -2593,7 +2559,7 @@
         <v>309</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
@@ -2607,7 +2573,7 @@
         <v>310</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>
@@ -2621,7 +2587,7 @@
         <v>311</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>10</v>
@@ -2635,7 +2601,7 @@
         <v>312</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>10</v>
@@ -2649,7 +2615,7 @@
         <v>313</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>10</v>
@@ -2663,7 +2629,7 @@
         <v>314</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>10</v>
@@ -2677,7 +2643,7 @@
         <v>315</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>10</v>
@@ -2691,7 +2657,7 @@
         <v>316</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>10</v>
@@ -2705,7 +2671,7 @@
         <v>317</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>10</v>
@@ -2719,7 +2685,7 @@
         <v>318</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>10</v>
@@ -2733,7 +2699,7 @@
         <v>319</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>10</v>
@@ -3432,7 +3398,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -3472,7 +3438,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -3488,7 +3454,7 @@
         <v>400</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -3502,7 +3468,7 @@
         <v>401</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -3516,7 +3482,7 @@
         <v>402</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -3530,7 +3496,7 @@
         <v>403</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -3544,7 +3510,7 @@
         <v>404</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -4390,7 +4356,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -4430,7 +4396,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4446,7 +4412,7 @@
         <v>600</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
@@ -4460,7 +4426,7 @@
         <v>601</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -4474,7 +4440,7 @@
         <v>602</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -4488,7 +4454,7 @@
         <v>603</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>79</v>
@@ -4502,7 +4468,7 @@
         <v>604</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -4516,7 +4482,7 @@
         <v>605</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
@@ -4530,7 +4496,7 @@
         <v>606</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>79</v>
@@ -4544,7 +4510,7 @@
         <v>607</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -4558,7 +4524,7 @@
         <v>608</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
@@ -4572,7 +4538,7 @@
         <v>609</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>79</v>
@@ -4586,7 +4552,7 @@
         <v>610</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
@@ -4600,7 +4566,7 @@
         <v>611</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>79</v>
@@ -4614,7 +4580,7 @@
         <v>612</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Changed nr for ENG and SOV general/navy ID's
</commit_message>
<xml_diff>
--- a/BICE modfile/Leader_ID.xlsx
+++ b/BICE modfile/Leader_ID.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="6540" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GER" sheetId="1" r:id="rId1"/>
     <sheet name="ENG" sheetId="4" r:id="rId2"/>
-    <sheet name="USA" sheetId="5" r:id="rId3"/>
-    <sheet name="SOV" sheetId="6" r:id="rId4"/>
+    <sheet name="SOV" sheetId="6" r:id="rId3"/>
+    <sheet name="USA" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -457,9 +457,6 @@
     <t>Truscott, Lucian</t>
   </si>
   <si>
-    <t>UNITED KINGDOM  600 - 799</t>
-  </si>
-  <si>
     <t>Zhukov, Georgy</t>
   </si>
   <si>
@@ -514,7 +511,10 @@
     <t>Resinged on 27 jan 1938</t>
   </si>
   <si>
-    <t>UNITED KINGDOM  300 - 700</t>
+    <t>UNITED KINGDOM  300 - 849</t>
+  </si>
+  <si>
+    <t>UNITED KINGDOM  850 - 1100</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -607,9 +607,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -647,9 +647,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -684,7 +684,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -719,7 +719,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -988,7 +988,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K4" s="2">
         <v>200</v>
@@ -1013,7 +1013,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K5" s="2">
         <v>201</v>
@@ -1419,7 +1419,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>10</v>
@@ -1442,13 +1442,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K24" s="2">
         <v>220</v>
@@ -2356,8 +2356,1029 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S103"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0">
+      <selection sqref="A1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>300</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>301</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>302</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>303</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>304</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>305</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>306</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>307</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>308</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>309</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>310</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>311</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>312</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>313</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>314</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>315</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>316</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>317</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>318</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>319</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>320</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>321</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>322</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>323</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>324</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>325</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>326</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>327</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>328</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>329</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>330</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>331</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>332</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>333</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>334</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>335</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>336</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>337</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>338</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>339</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>340</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>341</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>342</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>343</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>344</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>345</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>346</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>347</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>348</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>349</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>350</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>351</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>352</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>353</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>354</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>355</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>356</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>357</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>358</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>359</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>360</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>361</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>362</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>363</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>364</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>365</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>366</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>367</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>368</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>369</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>370</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>371</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>372</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>373</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>374</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>375</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>376</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>377</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>378</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>379</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>380</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>381</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>382</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>383</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>384</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>385</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>386</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>387</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>388</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>389</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>390</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>391</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>392</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>393</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>394</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>395</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>396</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>397</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>398</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>399</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S107"/>
+  <sheetViews>
+    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2405,13 +3426,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2425,18 +3446,18 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="O3" s="5"/>
+      <c r="O3" s="6"/>
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2444,10 +3465,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>301</v>
+        <v>601</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -2458,10 +3479,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>302</v>
+        <v>602</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -2472,13 +3493,13 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>303</v>
+        <v>603</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -2486,10 +3507,10 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>304</v>
+        <v>604</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -2500,13 +3521,13 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>305</v>
+        <v>605</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -2514,13 +3535,13 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>306</v>
+        <v>606</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -2528,10 +3549,10 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>307</v>
+        <v>607</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -2542,10 +3563,10 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>308</v>
+        <v>608</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
@@ -2556,13 +3577,13 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>309</v>
+        <v>609</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -2570,13 +3591,13 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>310</v>
+        <v>610</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -2584,13 +3605,13 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>311</v>
+        <v>611</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -2598,10 +3619,10 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>312</v>
+        <v>612</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>10</v>
@@ -2612,105 +3633,70 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>313</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>613</v>
+      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>314</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>614</v>
+      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>315</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>615</v>
+      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>316</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>616</v>
+      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>317</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>617</v>
+      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>318</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>618</v>
+      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>319</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>619</v>
+      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>320</v>
+        <v>620</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2719,7 +3705,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>321</v>
+        <v>621</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2728,7 +3714,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>322</v>
+        <v>622</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2737,7 +3723,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>323</v>
+        <v>623</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2746,7 +3732,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>324</v>
+        <v>624</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2755,7 +3741,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>325</v>
+        <v>625</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2764,7 +3750,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>326</v>
+        <v>626</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2773,7 +3759,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>327</v>
+        <v>627</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -2782,7 +3768,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>328</v>
+        <v>628</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2791,7 +3777,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>329</v>
+        <v>629</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2800,7 +3786,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>330</v>
+        <v>630</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2809,7 +3795,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>331</v>
+        <v>631</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2818,7 +3804,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>332</v>
+        <v>632</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2827,7 +3813,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>333</v>
+        <v>633</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2836,7 +3822,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>334</v>
+        <v>634</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2845,7 +3831,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>335</v>
+        <v>635</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2853,7 +3839,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>336</v>
+        <v>636</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2861,7 +3847,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>337</v>
+        <v>637</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2869,7 +3855,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>338</v>
+        <v>638</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2877,7 +3863,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>339</v>
+        <v>639</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2885,7 +3871,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>340</v>
+        <v>640</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2893,7 +3879,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>341</v>
+        <v>641</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2901,7 +3887,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>342</v>
+        <v>642</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2909,7 +3895,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>343</v>
+        <v>643</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2917,7 +3903,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>344</v>
+        <v>644</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2925,7 +3911,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>345</v>
+        <v>645</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2933,7 +3919,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>346</v>
+        <v>646</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2941,7 +3927,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>347</v>
+        <v>647</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2949,7 +3935,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>348</v>
+        <v>648</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -2957,7 +3943,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>349</v>
+        <v>649</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -2965,7 +3951,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>350</v>
+        <v>650</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2973,7 +3959,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>351</v>
+        <v>651</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2981,7 +3967,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>352</v>
+        <v>652</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2989,7 +3975,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>353</v>
+        <v>653</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2997,7 +3983,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>354</v>
+        <v>654</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -3005,7 +3991,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>355</v>
+        <v>655</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -3013,7 +3999,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>356</v>
+        <v>656</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -3021,7 +4007,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>357</v>
+        <v>657</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -3029,7 +4015,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>358</v>
+        <v>658</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -3037,7 +4023,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>359</v>
+        <v>659</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -3045,7 +4031,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>360</v>
+        <v>660</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -3053,7 +4039,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>361</v>
+        <v>661</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -3061,7 +4047,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>362</v>
+        <v>662</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -3069,7 +4055,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>363</v>
+        <v>663</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -3077,7 +4063,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>364</v>
+        <v>664</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -3085,7 +4071,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>365</v>
+        <v>665</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -3093,7 +4079,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>366</v>
+        <v>666</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -3101,7 +4087,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>367</v>
+        <v>667</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -3109,7 +4095,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>368</v>
+        <v>668</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -3117,7 +4103,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>369</v>
+        <v>669</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -3125,7 +4111,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>370</v>
+        <v>670</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -3133,7 +4119,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>371</v>
+        <v>671</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -3141,7 +4127,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>372</v>
+        <v>672</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -3149,7 +4135,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>373</v>
+        <v>673</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -3157,7 +4143,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>374</v>
+        <v>674</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -3165,7 +4151,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>375</v>
+        <v>675</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -3173,7 +4159,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>376</v>
+        <v>676</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -3181,7 +4167,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>377</v>
+        <v>677</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -3189,7 +4175,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>378</v>
+        <v>678</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -3197,7 +4183,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>379</v>
+        <v>679</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -3205,7 +4191,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>380</v>
+        <v>680</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -3213,7 +4199,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>381</v>
+        <v>681</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -3221,7 +4207,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>382</v>
+        <v>682</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -3229,7 +4215,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>383</v>
+        <v>683</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -3237,7 +4223,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>384</v>
+        <v>684</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -3245,7 +4231,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>385</v>
+        <v>685</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -3253,7 +4239,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>386</v>
+        <v>686</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -3261,7 +4247,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>387</v>
+        <v>687</v>
       </c>
       <c r="B91" s="3"/>
       <c r="D91" s="2"/>
@@ -3270,7 +4256,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>388</v>
+        <v>688</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -3278,7 +4264,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>389</v>
+        <v>689</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -3286,7 +4272,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>390</v>
+        <v>690</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -3294,7 +4280,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>391</v>
+        <v>691</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -3302,7 +4288,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>392</v>
+        <v>692</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -3310,7 +4296,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>393</v>
+        <v>693</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -3318,7 +4304,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>394</v>
+        <v>694</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -3326,7 +4312,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>395</v>
+        <v>695</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -3334,7 +4320,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>396</v>
+        <v>696</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -3342,7 +4328,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>397</v>
+        <v>697</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -3350,7 +4336,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>398</v>
+        <v>698</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -3358,11 +4344,23 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>399</v>
+        <v>699</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3373,7 +4371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S107"/>
   <sheetViews>
@@ -4329,1002 +5327,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S107"/>
-  <sheetViews>
-    <sheetView showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>600</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>601</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>602</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>603</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>604</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>605</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>606</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>607</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>608</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>609</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>610</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>611</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>612</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>613</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>614</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>615</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>616</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>617</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>618</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>619</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>620</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>621</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>622</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>623</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>624</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>625</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>626</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>627</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>628</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>629</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>630</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>631</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>632</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>633</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>634</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>635</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>636</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>637</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>638</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>639</v>
-      </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>640</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>641</v>
-      </c>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>642</v>
-      </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>643</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>644</v>
-      </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>645</v>
-      </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>646</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>647</v>
-      </c>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>648</v>
-      </c>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>649</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>650</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>651</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
-        <v>652</v>
-      </c>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
-        <v>653</v>
-      </c>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>654</v>
-      </c>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>655</v>
-      </c>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>656</v>
-      </c>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>657</v>
-      </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>658</v>
-      </c>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>659</v>
-      </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>660</v>
-      </c>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>661</v>
-      </c>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>662</v>
-      </c>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
-        <v>663</v>
-      </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
-        <v>664</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
-        <v>665</v>
-      </c>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>666</v>
-      </c>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
-        <v>667</v>
-      </c>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
-        <v>668</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
-        <v>669</v>
-      </c>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
-        <v>670</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
-        <v>671</v>
-      </c>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
-        <v>672</v>
-      </c>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
-        <v>673</v>
-      </c>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
-        <v>674</v>
-      </c>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
-        <v>675</v>
-      </c>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
-        <v>676</v>
-      </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
-        <v>677</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
-        <v>678</v>
-      </c>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
-        <v>679</v>
-      </c>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
-        <v>680</v>
-      </c>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
-        <v>681</v>
-      </c>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
-        <v>682</v>
-      </c>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
-        <v>683</v>
-      </c>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
-        <v>684</v>
-      </c>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
-        <v>685</v>
-      </c>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>686</v>
-      </c>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
-        <v>687</v>
-      </c>
-      <c r="B91" s="3"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
-        <v>688</v>
-      </c>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
-        <v>689</v>
-      </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
-        <v>690</v>
-      </c>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
-        <v>691</v>
-      </c>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
-        <v>692</v>
-      </c>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
-        <v>693</v>
-      </c>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
-        <v>694</v>
-      </c>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
-        <v>695</v>
-      </c>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
-        <v>696</v>
-      </c>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
-        <v>697</v>
-      </c>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
-        <v>698</v>
-      </c>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
-        <v>699</v>
-      </c>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="2"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="2"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="2"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
SOV country file done FRA country file WIP
</commit_message>
<xml_diff>
--- a/BICE modfile/Leader_ID.xlsx
+++ b/BICE modfile/Leader_ID.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="8640" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GER" sheetId="1" r:id="rId1"/>
     <sheet name="ENG" sheetId="4" r:id="rId2"/>
     <sheet name="SOV" sheetId="6" r:id="rId3"/>
-    <sheet name="USA" sheetId="5" r:id="rId4"/>
+    <sheet name="FRA" sheetId="5" r:id="rId4"/>
+    <sheet name="USA (2)" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="167">
   <si>
     <t>ID</t>
   </si>
@@ -514,13 +515,16 @@
     <t>UNITED KINGDOM  300 - 849</t>
   </si>
   <si>
-    <t>UNITED KINGDOM  850 - 1100</t>
+    <t>SOVIET UNION  850 - 999</t>
+  </si>
+  <si>
+    <t>FRANCE 1000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -571,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -586,6 +590,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,7 +616,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -647,7 +654,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -682,6 +689,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -717,9 +741,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -915,28 +956,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="K1" s="8" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -2376,17 +2417,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -3374,6 +3415,1004 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S107"/>
+  <sheetViews>
+    <sheetView showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>600</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>601</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>602</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>603</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>604</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>605</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>606</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>607</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>608</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>609</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>610</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>611</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>612</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>613</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>614</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>615</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>616</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>617</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>618</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>619</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>620</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>621</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>622</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>623</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>624</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>625</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>626</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>627</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>628</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>629</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>630</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>631</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>632</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>633</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>634</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>635</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>636</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>637</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>638</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>639</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>640</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>641</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>642</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>643</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>644</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>645</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>646</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>647</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>648</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>649</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>650</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>651</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>652</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>653</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>654</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>655</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>656</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>657</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>658</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>659</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>660</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>661</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>662</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>663</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>664</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>665</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>666</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>667</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>668</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>669</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>670</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>671</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>672</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>673</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>674</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>675</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>676</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>677</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>678</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>679</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>680</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>681</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>682</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>683</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>684</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>685</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>686</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>687</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>688</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>689</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>690</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>691</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>692</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>693</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>694</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>695</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>696</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>697</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>698</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>699</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S107"/>
   <sheetViews>
@@ -3397,17 +4436,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="A1" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -3451,13 +4490,13 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -3465,10 +4504,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>601</v>
+        <v>401</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -3479,10 +4518,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>602</v>
+        <v>402</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -3493,13 +4532,13 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>603</v>
+        <v>403</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -3507,10 +4546,10 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>604</v>
+        <v>404</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -3521,119 +4560,79 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>605</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>606</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>607</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>608</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>609</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>409</v>
+      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>610</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>611</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>612</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>412</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>613</v>
+        <v>413</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3642,7 +4641,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>614</v>
+        <v>414</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -3651,7 +4650,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>615</v>
+        <v>415</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -3660,7 +4659,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>616</v>
+        <v>416</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -3669,7 +4668,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>617</v>
+        <v>417</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -3678,7 +4677,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>618</v>
+        <v>418</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -3687,7 +4686,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>619</v>
+        <v>419</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -3696,7 +4695,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>620</v>
+        <v>420</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -3705,7 +4704,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>621</v>
+        <v>421</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -3714,7 +4713,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>622</v>
+        <v>422</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -3723,7 +4722,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>623</v>
+        <v>423</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -3732,7 +4731,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>624</v>
+        <v>424</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -3741,7 +4740,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>625</v>
+        <v>425</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -3750,7 +4749,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>626</v>
+        <v>426</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -3759,7 +4758,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>627</v>
+        <v>427</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -3768,7 +4767,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>628</v>
+        <v>428</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -3777,7 +4776,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>629</v>
+        <v>429</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -3786,7 +4785,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>630</v>
+        <v>430</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -3795,7 +4794,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>631</v>
+        <v>431</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -3804,7 +4803,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>632</v>
+        <v>432</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -3813,7 +4812,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>633</v>
+        <v>433</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -3822,7 +4821,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>634</v>
+        <v>434</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -3831,7 +4830,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>635</v>
+        <v>435</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -3839,7 +4838,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>636</v>
+        <v>436</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -3847,7 +4846,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>637</v>
+        <v>437</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -3855,7 +4854,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>638</v>
+        <v>438</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -3863,7 +4862,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>639</v>
+        <v>439</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -3871,7 +4870,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>640</v>
+        <v>440</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -3879,7 +4878,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>641</v>
+        <v>441</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -3887,7 +4886,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>642</v>
+        <v>442</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -3895,7 +4894,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>643</v>
+        <v>443</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -3903,7 +4902,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>644</v>
+        <v>444</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -3911,7 +4910,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>645</v>
+        <v>445</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -3919,7 +4918,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>646</v>
+        <v>446</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -3927,7 +4926,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>647</v>
+        <v>447</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -3935,7 +4934,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>648</v>
+        <v>448</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -3943,7 +4942,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>649</v>
+        <v>449</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -3951,7 +4950,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>650</v>
+        <v>450</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -3959,7 +4958,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>651</v>
+        <v>451</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -3967,7 +4966,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>652</v>
+        <v>452</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -3975,7 +4974,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>653</v>
+        <v>453</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -3983,7 +4982,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>654</v>
+        <v>454</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -3991,7 +4990,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>655</v>
+        <v>455</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -3999,7 +4998,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>656</v>
+        <v>456</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -4007,7 +5006,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>657</v>
+        <v>457</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -4015,7 +5014,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>658</v>
+        <v>458</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -4023,7 +5022,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>659</v>
+        <v>459</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -4031,7 +5030,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>660</v>
+        <v>460</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -4039,7 +5038,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>661</v>
+        <v>461</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -4047,7 +5046,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>662</v>
+        <v>462</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -4055,7 +5054,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>663</v>
+        <v>463</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -4063,7 +5062,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>664</v>
+        <v>464</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -4071,7 +5070,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>665</v>
+        <v>465</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -4079,7 +5078,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>666</v>
+        <v>466</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -4087,7 +5086,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>667</v>
+        <v>467</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -4095,7 +5094,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>668</v>
+        <v>468</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -4103,7 +5102,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>669</v>
+        <v>469</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -4111,7 +5110,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>670</v>
+        <v>470</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -4119,7 +5118,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>671</v>
+        <v>471</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -4127,7 +5126,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>672</v>
+        <v>472</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -4135,7 +5134,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>673</v>
+        <v>473</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -4143,7 +5142,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>674</v>
+        <v>474</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -4151,7 +5150,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>675</v>
+        <v>475</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -4159,7 +5158,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>676</v>
+        <v>476</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -4167,7 +5166,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>677</v>
+        <v>477</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -4175,7 +5174,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>678</v>
+        <v>478</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -4183,7 +5182,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>679</v>
+        <v>479</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -4191,7 +5190,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>680</v>
+        <v>480</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -4199,7 +5198,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>681</v>
+        <v>481</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -4207,7 +5206,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>682</v>
+        <v>482</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -4215,7 +5214,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>683</v>
+        <v>483</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -4223,7 +5222,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>684</v>
+        <v>484</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -4231,7 +5230,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>685</v>
+        <v>485</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -4239,7 +5238,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>686</v>
+        <v>486</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -4247,7 +5246,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>687</v>
+        <v>487</v>
       </c>
       <c r="B91" s="3"/>
       <c r="D91" s="2"/>
@@ -4256,7 +5255,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>688</v>
+        <v>488</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -4264,7 +5263,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>689</v>
+        <v>489</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -4272,7 +5271,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>690</v>
+        <v>490</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -4280,7 +5279,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>691</v>
+        <v>491</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -4288,7 +5287,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>692</v>
+        <v>492</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -4296,7 +5295,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>693</v>
+        <v>493</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -4304,7 +5303,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>694</v>
+        <v>494</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -4312,7 +5311,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>695</v>
+        <v>495</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -4320,7 +5319,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>696</v>
+        <v>496</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -4328,7 +5327,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>697</v>
+        <v>497</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -4336,7 +5335,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>698</v>
+        <v>498</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -4344,7 +5343,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>699</v>
+        <v>499</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -4371,7 +5370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S107"/>
   <sheetViews>
@@ -4395,17 +5394,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -4424,13 +5423,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4444,7 +5443,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="O3" s="6"/>
+      <c r="O3" s="8"/>
       <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added JAP and ITA country-files Corrected some typos Added new MAN-decisions
</commit_message>
<xml_diff>
--- a/BICE modfile/Leader_ID.xlsx
+++ b/BICE modfile/Leader_ID.xlsx
@@ -4,21 +4,24 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="8640" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="GER" sheetId="1" r:id="rId1"/>
     <sheet name="ENG" sheetId="4" r:id="rId2"/>
     <sheet name="SOV" sheetId="6" r:id="rId3"/>
     <sheet name="FRA" sheetId="5" r:id="rId4"/>
-    <sheet name="USA (2)" sheetId="7" r:id="rId5"/>
+    <sheet name="ITA" sheetId="8" r:id="rId5"/>
+    <sheet name="JAP" sheetId="9" r:id="rId6"/>
+    <sheet name="USA" sheetId="7" r:id="rId7"/>
+    <sheet name="ROM" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="211">
   <si>
     <t>ID</t>
   </si>
@@ -518,7 +521,139 @@
     <t>SOVIET UNION  850 - 999</t>
   </si>
   <si>
-    <t>FRANCE 1000</t>
+    <t>Weygand, Maxime</t>
+  </si>
+  <si>
+    <t>Gamelin, Maurice</t>
+  </si>
+  <si>
+    <t>Georges, Alphonse</t>
+  </si>
+  <si>
+    <t>Ardant du Picq, Charles</t>
+  </si>
+  <si>
+    <t>FRANCE 1000 1499</t>
+  </si>
+  <si>
+    <t>Badoglio, Pietro</t>
+  </si>
+  <si>
+    <t>Bono, Emilio De</t>
+  </si>
+  <si>
+    <t>Graziani, Rodolfo</t>
+  </si>
+  <si>
+    <t>Duca di Bergamo, Adalberto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Albert, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ago, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambrosio, </t>
+  </si>
+  <si>
+    <t>Duca degli Abruzzi, Amedeo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amico, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antonelli, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ardito, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arena, </t>
+  </si>
+  <si>
+    <t>Armellini, Q.</t>
+  </si>
+  <si>
+    <t>Bernezzo, Asinari di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babini, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burzagli, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baistrocchi, </t>
+  </si>
+  <si>
+    <t>Balbo, Italo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balisti, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balocco, </t>
+  </si>
+  <si>
+    <t>Prun, Barbasetti di</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barbieri, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basso, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bastico, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battisti, </t>
+  </si>
+  <si>
+    <t>Pralormo, Beraudo di</t>
+  </si>
+  <si>
+    <t>Bergonzoli, B.</t>
+  </si>
+  <si>
+    <t>Bergonzoli, A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bettoni, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bianchi, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bignani, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brunetti, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruno, </t>
+  </si>
+  <si>
+    <t>FRANCE 1500 - 1699</t>
+  </si>
+  <si>
+    <t>FRANCE 1700 - 1999</t>
+  </si>
+  <si>
+    <t>Terauchi, Hisaichi</t>
+  </si>
+  <si>
+    <t>Hata, Shunroku</t>
+  </si>
+  <si>
+    <t>Matsui, Iwane</t>
+  </si>
+  <si>
+    <t>Yamashita, Tomoyuki</t>
+  </si>
+  <si>
+    <t>Muto, Akira</t>
   </si>
 </sst>
 </file>
@@ -4416,8 +4551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4437,7 +4572,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -4490,10 +4625,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -4504,10 +4639,10 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>401</v>
+        <v>1001</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
@@ -4518,13 +4653,13 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>402</v>
+        <v>1002</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -4532,10 +4667,10 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>403</v>
+        <v>1003</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -4546,21 +4681,16 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>404</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>1004</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>405</v>
+        <v>1005</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -4569,7 +4699,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>406</v>
+        <v>1006</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -4578,7 +4708,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>407</v>
+        <v>1007</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -4587,7 +4717,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>408</v>
+        <v>1008</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -4596,7 +4726,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>409</v>
+        <v>1009</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -4605,7 +4735,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>410</v>
+        <v>1010</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -4614,7 +4744,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>411</v>
+        <v>1011</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -4623,7 +4753,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>412</v>
+        <v>1012</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -4632,7 +4762,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>413</v>
+        <v>1013</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -4641,7 +4771,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>414</v>
+        <v>1014</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -4650,7 +4780,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>415</v>
+        <v>1015</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -4659,7 +4789,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>416</v>
+        <v>1016</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -4668,7 +4798,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>417</v>
+        <v>1017</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -4677,7 +4807,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>418</v>
+        <v>1018</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -4686,7 +4816,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>419</v>
+        <v>1019</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -4695,7 +4825,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>420</v>
+        <v>1020</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -4704,7 +4834,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>421</v>
+        <v>1021</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -4713,7 +4843,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>422</v>
+        <v>1022</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -4722,7 +4852,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>423</v>
+        <v>1023</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -4731,7 +4861,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>424</v>
+        <v>1024</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -4740,7 +4870,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>425</v>
+        <v>1025</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -4749,7 +4879,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>426</v>
+        <v>1026</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -4758,7 +4888,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>427</v>
+        <v>1027</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -4767,7 +4897,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>428</v>
+        <v>1028</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -4776,7 +4906,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>429</v>
+        <v>1029</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -4785,7 +4915,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>430</v>
+        <v>1030</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -4794,7 +4924,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>431</v>
+        <v>1031</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -4803,7 +4933,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>432</v>
+        <v>1032</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -4812,7 +4942,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>433</v>
+        <v>1033</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -4821,7 +4951,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>434</v>
+        <v>1034</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -4830,7 +4960,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>435</v>
+        <v>1035</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -4838,7 +4968,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>436</v>
+        <v>1036</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -4846,7 +4976,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>437</v>
+        <v>1037</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -4854,7 +4984,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>438</v>
+        <v>1038</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -4862,7 +4992,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>439</v>
+        <v>1039</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -4870,7 +5000,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>440</v>
+        <v>1040</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -4878,7 +5008,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>441</v>
+        <v>1041</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -4886,7 +5016,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>442</v>
+        <v>1042</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -4894,7 +5024,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>443</v>
+        <v>1043</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -4902,7 +5032,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>444</v>
+        <v>1044</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -4910,7 +5040,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>445</v>
+        <v>1045</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -4918,7 +5048,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>446</v>
+        <v>1046</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -4926,7 +5056,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>447</v>
+        <v>1047</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -4934,7 +5064,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>448</v>
+        <v>1048</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -4942,7 +5072,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>449</v>
+        <v>1049</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -4950,7 +5080,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>450</v>
+        <v>1050</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -4958,7 +5088,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>451</v>
+        <v>1051</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -4966,7 +5096,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>452</v>
+        <v>1052</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -4974,7 +5104,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>453</v>
+        <v>1053</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -4982,7 +5112,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>454</v>
+        <v>1054</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -4990,7 +5120,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>455</v>
+        <v>1055</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -4998,7 +5128,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>456</v>
+        <v>1056</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -5006,7 +5136,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>457</v>
+        <v>1057</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -5014,7 +5144,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>458</v>
+        <v>1058</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -5022,7 +5152,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>459</v>
+        <v>1059</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -5030,7 +5160,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>460</v>
+        <v>1060</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -5038,7 +5168,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>461</v>
+        <v>1061</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -5046,7 +5176,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>462</v>
+        <v>1062</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -5054,7 +5184,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>463</v>
+        <v>1063</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -5062,7 +5192,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>464</v>
+        <v>1064</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -5070,7 +5200,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>465</v>
+        <v>1065</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -5078,7 +5208,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>466</v>
+        <v>1066</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -5086,7 +5216,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>467</v>
+        <v>1067</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -5094,7 +5224,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>468</v>
+        <v>1068</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -5102,7 +5232,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>469</v>
+        <v>1069</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -5110,7 +5240,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>470</v>
+        <v>1070</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -5118,7 +5248,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>471</v>
+        <v>1071</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -5126,7 +5256,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>472</v>
+        <v>1072</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -5134,7 +5264,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>473</v>
+        <v>1073</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -5142,7 +5272,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>474</v>
+        <v>1074</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -5150,7 +5280,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>475</v>
+        <v>1075</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -5158,7 +5288,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>476</v>
+        <v>1076</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -5166,7 +5296,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>477</v>
+        <v>1077</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -5174,7 +5304,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>478</v>
+        <v>1078</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -5182,7 +5312,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>479</v>
+        <v>1079</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -5190,7 +5320,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>480</v>
+        <v>1080</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -5198,7 +5328,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>481</v>
+        <v>1081</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -5206,7 +5336,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>482</v>
+        <v>1082</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -5214,7 +5344,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>483</v>
+        <v>1083</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -5222,7 +5352,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>484</v>
+        <v>1084</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -5230,7 +5360,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>485</v>
+        <v>1085</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -5238,7 +5368,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>486</v>
+        <v>1086</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -5246,7 +5376,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>487</v>
+        <v>1087</v>
       </c>
       <c r="B91" s="3"/>
       <c r="D91" s="2"/>
@@ -5255,7 +5385,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>488</v>
+        <v>1088</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -5263,7 +5393,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>489</v>
+        <v>1089</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -5271,7 +5401,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>490</v>
+        <v>1090</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -5279,7 +5409,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>491</v>
+        <v>1091</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -5287,7 +5417,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>492</v>
+        <v>1092</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -5295,7 +5425,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>493</v>
+        <v>1093</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -5303,7 +5433,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>494</v>
+        <v>1094</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -5311,7 +5441,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>495</v>
+        <v>1095</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -5319,7 +5449,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>496</v>
+        <v>1096</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -5327,7 +5457,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>497</v>
+        <v>1097</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -5335,7 +5465,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>498</v>
+        <v>1098</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -5343,7 +5473,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>499</v>
+        <v>1099</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -5371,6 +5501,1104 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S107"/>
+  <sheetViews>
+    <sheetView showRowColHeaders="0" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1500</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1501</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1502</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1503</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1504</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1505</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1506</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1507</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1508</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1509</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1510</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1511</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1512</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>1513</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>1514</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>1515</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>1516</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1517</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1518</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>1519</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>1520</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>1521</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>1522</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>1523</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>1524</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>1525</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>1526</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>1527</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>1528</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1529</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>1530</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>1531</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>1532</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>1533</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>1534</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>1535</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>1536</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>1537</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>1538</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>1539</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>1540</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>1541</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>1542</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>1543</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>1544</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>1545</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>1546</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>1547</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>1548</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>1549</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>1550</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>1551</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>1552</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>1553</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>1554</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>1555</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>1556</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>1557</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>1558</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>1559</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>1560</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>1561</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>1562</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>1563</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>1564</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>1565</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>1566</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>1567</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>1568</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>1569</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>1570</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>1571</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>1572</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>1573</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>1574</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>1575</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>1576</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>1577</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>1578</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>1579</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>1580</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>1581</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>1582</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>1583</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>1584</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>1585</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>1586</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>1587</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>1588</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>1589</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>1590</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>1591</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>1592</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>1593</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>1594</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>1595</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>1596</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>1597</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>1598</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>1599</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S107"/>
   <sheetViews>
@@ -5395,7 +6623,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>140</v>
+        <v>205</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -5448,6 +6676,1922 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
+        <v>1700</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1701</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1702</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1703</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1704</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1705</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1706</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1707</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1708</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1709</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1710</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1711</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1712</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>1713</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>1714</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>1715</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>1716</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1717</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1718</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>1719</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>1720</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>1721</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>1722</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>1723</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>1724</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>1725</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>1726</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>1727</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>1728</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1729</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>1730</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>1731</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>1732</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>1733</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>1734</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>1735</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>1736</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>1737</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>1738</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>1739</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>1740</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>1741</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>1742</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>1743</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>1744</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>1745</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>1746</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>1747</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>1748</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>1749</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>1750</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>1751</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>1752</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>1753</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>1754</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>1755</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>1756</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>1757</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>1758</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>1759</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>1760</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>1761</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>1762</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>1763</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>1764</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>1765</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>1766</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>1767</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>1768</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>1769</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>1770</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>1771</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>1772</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>1773</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>1774</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>1775</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>1776</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>1777</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>1778</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>1779</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>1780</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>1781</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>1782</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>1783</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>1784</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>1785</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>1786</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>1787</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>1788</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>1789</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>1790</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>1791</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>1792</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>1793</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>1794</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>1795</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>1796</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>1797</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>1798</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>1799</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S107"/>
+  <sheetViews>
+    <sheetView showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>400</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>401</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>402</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>403</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>404</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>405</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>406</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>407</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>408</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>409</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>410</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>411</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>412</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>413</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>414</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>415</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>416</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>417</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>418</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>419</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>420</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>421</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>422</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>423</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>424</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>425</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>426</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>427</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>428</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>429</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>430</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>431</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>432</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>433</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>434</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>435</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>436</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>437</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>438</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>439</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>440</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>441</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>442</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>443</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>444</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>445</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>446</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>447</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>448</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>449</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>450</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>451</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>452</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>453</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>454</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>455</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>456</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>457</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>458</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>459</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>460</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>461</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>462</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>463</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>464</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>465</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>466</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>467</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>468</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>469</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>470</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>471</v>
+      </c>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>472</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>473</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>474</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>475</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>476</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>477</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>478</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>479</v>
+      </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>480</v>
+      </c>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>481</v>
+      </c>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>482</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>483</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>484</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>485</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>486</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>487</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>488</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>489</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>490</v>
+      </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>491</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>492</v>
+      </c>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>493</v>
+      </c>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>494</v>
+      </c>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>495</v>
+      </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>496</v>
+      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>497</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>498</v>
+      </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>499</v>
+      </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S107"/>
+  <sheetViews>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="32.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>400</v>
       </c>
       <c r="B4" s="1" t="s">

</xml_diff>

<commit_message>
Added HUN and Horthy to leader spreadsheet
</commit_message>
<xml_diff>
--- a/BICE modfile/Leader_ID.xlsx
+++ b/BICE modfile/Leader_ID.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0E521F21-3F7E-4BE6-B30F-86907F430DC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="11"/>
+    <workbookView xWindow="14940" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Landcode" sheetId="11" r:id="rId1"/>
@@ -20,14 +21,14 @@
     <sheet name="YUN" sheetId="13" r:id="rId11"/>
     <sheet name="SHX" sheetId="14" r:id="rId12"/>
     <sheet name="GXC" sheetId="15" r:id="rId13"/>
+    <sheet name="HUN" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="419">
   <si>
     <t>ID</t>
   </si>
@@ -1275,12 +1276,21 @@
   </si>
   <si>
     <t>Li Zongren</t>
+  </si>
+  <si>
+    <t>HUNGARY  3200 - 3399</t>
+  </si>
+  <si>
+    <t>Regent Miklós Horthy  (absolutism)</t>
+  </si>
+  <si>
+    <t>Regent Miklós Horthy  (fasism)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1331,7 +1341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1355,6 +1365,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1700,7 +1713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2320,7 +2333,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:S107"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -2343,17 +2356,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>399</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -3250,7 +3263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3273,17 +3286,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>411</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -4035,792 +4048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S107"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2900</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>2901</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>2902</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>2903</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>2904</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>2905</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>2906</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>2907</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>2908</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>2909</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>2910</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2911</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>2912</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>2913</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>2914</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>2915</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>2916</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>2917</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>2918</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>2919</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>2920</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>2921</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="K29" s="2"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="K30" s="2"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="K35" s="2"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="K36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="K37" s="2"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="K38" s="2"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
-      <c r="D74" s="2">
-        <f ca="1">A4:D74</f>
-        <v>0</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
-      <c r="B91" s="3"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="2"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="2"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="2"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:S107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4843,17 +4071,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>414</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="A1" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -4897,13 +4125,13 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>3000</v>
+        <v>2900</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -4911,7 +4139,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>3001</v>
+        <v>2901</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -4920,7 +4148,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>3002</v>
+        <v>2902</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -4929,7 +4157,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>3003</v>
+        <v>2903</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -4938,7 +4166,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>3004</v>
+        <v>2904</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -4947,7 +4175,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>3005</v>
+        <v>2905</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -4956,7 +4184,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>3006</v>
+        <v>2906</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -4965,7 +4193,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>3007</v>
+        <v>2907</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -4974,7 +4202,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>3008</v>
+        <v>2908</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -4983,7 +4211,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>3009</v>
+        <v>2909</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -4992,7 +4220,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>3010</v>
+        <v>2910</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -5001,7 +4229,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>3011</v>
+        <v>2911</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -5010,7 +4238,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>3012</v>
+        <v>2912</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -5019,7 +4247,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>3013</v>
+        <v>2913</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -5028,7 +4256,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>3014</v>
+        <v>2914</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -5037,7 +4265,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>3015</v>
+        <v>2915</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -5046,7 +4274,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>3016</v>
+        <v>2916</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -5055,7 +4283,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>3017</v>
+        <v>2917</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -5064,7 +4292,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>3018</v>
+        <v>2918</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -5073,7 +4301,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>3019</v>
+        <v>2919</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -5082,7 +4310,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>3020</v>
+        <v>2920</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -5091,7 +4319,1582 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
+        <v>2921</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="D74" s="2">
+        <f ca="1">A4:D74</f>
+        <v>0</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:S107"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3000</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3001</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3002</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3003</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3004</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>3005</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>3006</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>3007</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>3008</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>3009</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>3010</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>3011</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3012</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3013</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>3014</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>3015</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>3016</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>3017</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>3018</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>3019</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>3020</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>3021</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="D74" s="2">
+        <f ca="1">A4:D74</f>
+        <v>0</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="2"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2"/>
+      <c r="B91" s="3"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC65246-6851-46E6-8B1F-063DBD75720C}">
+  <dimension ref="A1:S107"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="3.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3200</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3201</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3202</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3203</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3204</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>3205</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>3206</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>3207</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>3208</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>3209</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>3210</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>3211</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3212</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3213</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>3214</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>3215</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>3216</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>3217</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>3218</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>3219</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>3220</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>3221</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -5605,7 +6408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5628,28 +6431,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -7066,7 +7869,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S103"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" topLeftCell="A13" workbookViewId="0">
@@ -7089,17 +7892,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -8087,11 +8890,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8110,17 +8913,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -8164,7 +8967,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>600</v>
+        <v>850</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>156</v>
@@ -8178,7 +8981,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>601</v>
+        <v>851</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>151</v>
@@ -8192,7 +8995,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>602</v>
+        <v>852</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>146</v>
@@ -8206,7 +9009,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>603</v>
+        <v>853</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>152</v>
@@ -8220,7 +9023,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>604</v>
+        <v>854</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>149</v>
@@ -8234,7 +9037,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>605</v>
+        <v>855</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>150</v>
@@ -8248,7 +9051,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>606</v>
+        <v>856</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>154</v>
@@ -8262,7 +9065,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>607</v>
+        <v>857</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>147</v>
@@ -8276,7 +9079,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>608</v>
+        <v>858</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>148</v>
@@ -8290,7 +9093,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>609</v>
+        <v>859</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>153</v>
@@ -8304,7 +9107,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>610</v>
+        <v>860</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>145</v>
@@ -8318,7 +9121,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>611</v>
+        <v>861</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>155</v>
@@ -8332,7 +9135,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>612</v>
+        <v>862</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>157</v>
@@ -8346,7 +9149,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>613</v>
+        <v>863</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -8355,7 +9158,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>614</v>
+        <v>864</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -8364,7 +9167,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>615</v>
+        <v>865</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -8373,7 +9176,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>616</v>
+        <v>866</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -8382,7 +9185,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>617</v>
+        <v>867</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -8391,7 +9194,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>618</v>
+        <v>868</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -8400,7 +9203,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>619</v>
+        <v>869</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -8409,7 +9212,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>620</v>
+        <v>870</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -8418,7 +9221,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>621</v>
+        <v>871</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -8427,7 +9230,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>622</v>
+        <v>872</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -8436,7 +9239,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>623</v>
+        <v>873</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -8445,7 +9248,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>624</v>
+        <v>874</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -8454,7 +9257,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>625</v>
+        <v>875</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -8463,7 +9266,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>626</v>
+        <v>876</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -8472,7 +9275,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>627</v>
+        <v>877</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -8481,7 +9284,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>628</v>
+        <v>878</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -8490,7 +9293,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>629</v>
+        <v>879</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -8499,7 +9302,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>630</v>
+        <v>880</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -8508,7 +9311,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>631</v>
+        <v>881</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -8517,7 +9320,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>632</v>
+        <v>882</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -8526,7 +9329,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>633</v>
+        <v>883</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -8535,7 +9338,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>634</v>
+        <v>884</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -8544,7 +9347,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>635</v>
+        <v>885</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -8552,7 +9355,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>636</v>
+        <v>886</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -8560,7 +9363,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>637</v>
+        <v>887</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -8568,7 +9371,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>638</v>
+        <v>888</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -8576,7 +9379,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>639</v>
+        <v>889</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -8584,7 +9387,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>640</v>
+        <v>890</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -8592,7 +9395,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>641</v>
+        <v>891</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -8600,7 +9403,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>642</v>
+        <v>892</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -8608,7 +9411,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>643</v>
+        <v>893</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -8616,7 +9419,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>644</v>
+        <v>894</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -8624,7 +9427,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>645</v>
+        <v>895</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -8632,7 +9435,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>646</v>
+        <v>896</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -8640,7 +9443,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>647</v>
+        <v>897</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -8648,7 +9451,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>648</v>
+        <v>898</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -8656,7 +9459,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>649</v>
+        <v>899</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -8664,7 +9467,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>650</v>
+        <v>900</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -8672,7 +9475,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>651</v>
+        <v>901</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -8680,7 +9483,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>652</v>
+        <v>902</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -8688,7 +9491,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>653</v>
+        <v>903</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -8696,7 +9499,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>654</v>
+        <v>904</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -8704,7 +9507,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>655</v>
+        <v>905</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -8712,7 +9515,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>656</v>
+        <v>906</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -8720,7 +9523,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>657</v>
+        <v>907</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -8728,7 +9531,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>658</v>
+        <v>908</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -8736,7 +9539,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>659</v>
+        <v>909</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -8744,7 +9547,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>660</v>
+        <v>910</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -8752,7 +9555,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>661</v>
+        <v>911</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -8760,7 +9563,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>662</v>
+        <v>912</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -8768,7 +9571,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>663</v>
+        <v>913</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -8776,7 +9579,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>664</v>
+        <v>914</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -8784,7 +9587,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>665</v>
+        <v>915</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -8792,7 +9595,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>666</v>
+        <v>916</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -8800,7 +9603,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>667</v>
+        <v>917</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -8808,7 +9611,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>668</v>
+        <v>918</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -8816,7 +9619,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>669</v>
+        <v>919</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -8824,7 +9627,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>670</v>
+        <v>920</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -8832,7 +9635,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>671</v>
+        <v>921</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -8840,7 +9643,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>672</v>
+        <v>922</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -8848,7 +9651,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>673</v>
+        <v>923</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -8856,7 +9659,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>674</v>
+        <v>924</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -8864,7 +9667,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>675</v>
+        <v>925</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
@@ -8872,7 +9675,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>676</v>
+        <v>926</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
@@ -8880,7 +9683,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>677</v>
+        <v>927</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
@@ -8888,7 +9691,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>678</v>
+        <v>928</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -8896,7 +9699,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>679</v>
+        <v>929</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -8904,7 +9707,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>680</v>
+        <v>930</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
@@ -8912,7 +9715,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>681</v>
+        <v>931</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
@@ -8920,7 +9723,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>682</v>
+        <v>932</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
@@ -8928,7 +9731,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>683</v>
+        <v>933</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
@@ -8936,7 +9739,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>684</v>
+        <v>934</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
@@ -8944,7 +9747,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>685</v>
+        <v>935</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -8952,7 +9755,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>686</v>
+        <v>936</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -8960,7 +9763,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>687</v>
+        <v>937</v>
       </c>
       <c r="B91" s="3"/>
       <c r="D91" s="2"/>
@@ -8969,7 +9772,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>688</v>
+        <v>938</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -8977,7 +9780,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>689</v>
+        <v>939</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -8985,7 +9788,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>690</v>
+        <v>940</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -8993,7 +9796,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>691</v>
+        <v>941</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -9001,7 +9804,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>692</v>
+        <v>942</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -9009,7 +9812,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>693</v>
+        <v>943</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -9017,7 +9820,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>694</v>
+        <v>944</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -9025,7 +9828,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>695</v>
+        <v>945</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -9033,7 +9836,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>696</v>
+        <v>946</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -9041,7 +9844,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>697</v>
+        <v>947</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -9049,7 +9852,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>698</v>
+        <v>948</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -9057,7 +9860,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>699</v>
+        <v>949</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -9085,7 +9888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S107"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" workbookViewId="0">
@@ -9108,17 +9911,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -10038,10 +10841,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" topLeftCell="A73" workbookViewId="0">
+    <sheetView showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -10061,17 +10864,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -11136,7 +11939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S107"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" workbookViewId="0">
@@ -11159,17 +11962,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -12094,7 +12897,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S108"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" workbookViewId="0">
@@ -12117,17 +12920,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -13392,10 +14195,10 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
@@ -13415,17 +14218,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>

</xml_diff>

<commit_message>
Fixed leaders ID in NF SOV_purge_stalinists
</commit_message>
<xml_diff>
--- a/BICE modfile/Leader_ID.xlsx
+++ b/BICE modfile/Leader_ID.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{338D1E7C-13D5-4E1B-BA56-F5622F4AF5D6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6BDEAF9B-1349-4314-8222-5F895590C897}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14940" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="429">
   <si>
     <t>ID</t>
   </si>
@@ -1284,6 +1284,36 @@
   </si>
   <si>
     <t>promotion.1</t>
+  </si>
+  <si>
+    <t>Chernyakhovsky, Ivan</t>
+  </si>
+  <si>
+    <t>Budyonny, Semyon</t>
+  </si>
+  <si>
+    <t>Nikolai Vatutin</t>
+  </si>
+  <si>
+    <t>Kulik, Grigory</t>
+  </si>
+  <si>
+    <t>Govorov, Leonid</t>
+  </si>
+  <si>
+    <t>Purkayev, Maksim</t>
+  </si>
+  <si>
+    <t>Popov, Markian</t>
+  </si>
+  <si>
+    <t>Malinovsky, Rodion</t>
+  </si>
+  <si>
+    <t>Reyter, Max</t>
+  </si>
+  <si>
+    <t>Zakharov, Georgiy</t>
   </si>
 </sst>
 </file>
@@ -8145,7 +8175,7 @@
   <dimension ref="A1:S107"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8402,7 +8432,12 @@
       <c r="A17" s="2">
         <v>863</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="B17" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="K17" s="2"/>
@@ -8411,7 +8446,12 @@
       <c r="A18" s="2">
         <v>864</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="B18" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="K18" s="2"/>
@@ -8420,7 +8460,12 @@
       <c r="A19" s="2">
         <v>865</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="B19" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="K19" s="2"/>
@@ -8429,7 +8474,12 @@
       <c r="A20" s="2">
         <v>866</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="B20" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="K20" s="2"/>
@@ -8438,7 +8488,12 @@
       <c r="A21" s="2">
         <v>867</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="K21" s="2"/>
@@ -8447,7 +8502,12 @@
       <c r="A22" s="2">
         <v>868</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="B22" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="K22" s="2"/>
@@ -8456,7 +8516,12 @@
       <c r="A23" s="2">
         <v>869</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="B23" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="K23" s="2"/>
@@ -8483,7 +8548,12 @@
       <c r="A26" s="2">
         <v>872</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="B26" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="K26" s="2"/>
@@ -8608,7 +8678,12 @@
       <c r="A40" s="2">
         <v>886</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="B40" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
     </row>
@@ -8624,7 +8699,12 @@
       <c r="A42" s="2">
         <v>888</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="B42" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
     </row>
@@ -8632,7 +8712,12 @@
       <c r="A43" s="2">
         <v>889</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="B43" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>

</xml_diff>